<commit_message>
development in TES class file
</commit_message>
<xml_diff>
--- a/TES Code Error Log.xlsx
+++ b/TES Code Error Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kadenplewe/GranularFunnelFlowModeling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\PhD Research\GranularFunnelFlowModeling\GitFiles\GranularFunnelFlowModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFF70D29-2721-2346-9FFD-DD2CC6E702D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A59DC3-E2EA-4A04-931B-7867C505C649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
   </bookViews>
   <sheets>
     <sheet name="FF Code Base" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Problem Description</t>
   </si>
@@ -55,6 +53,21 @@
   </si>
   <si>
     <t>The outer steel shell was set to be the inner-most layer</t>
+  </si>
+  <si>
+    <t>Relevant Code</t>
+  </si>
+  <si>
+    <t>FF_test.m</t>
+  </si>
+  <si>
+    <t>Instability durring simulation, originating from oscilations at the wall and base</t>
+  </si>
+  <si>
+    <t>The scaling associated with transfering data from wall/base to the particle domain was incorrect. Initial scaling should use prototype parameters and the scaling used to transfer information to particle domain should use the model parameters.</t>
+  </si>
+  <si>
+    <t>TES.m, FF.m</t>
   </si>
 </sst>
 </file>
@@ -410,19 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C52C9A-ABED-8249-94C9-614CBC84848F}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.83203125" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
+    <col min="2" max="2" width="68.875" customWidth="1"/>
+    <col min="3" max="3" width="73.375" customWidth="1"/>
+    <col min="5" max="5" width="16.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -435,8 +449,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44786</v>
       </c>
@@ -448,6 +465,26 @@
       </c>
       <c r="D2" s="1">
         <v>44789</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44795</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44795</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -461,7 +498,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,7 +512,7 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
working on issues in TES.m
</commit_message>
<xml_diff>
--- a/TES Code Error Log.xlsx
+++ b/TES Code Error Log.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\PhD Research\GranularFunnelFlowModeling\GitFiles\GranularFunnelFlowModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A59DC3-E2EA-4A04-931B-7867C505C649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD0EFF7-90C4-4260-806C-4779FD8A7ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
   </bookViews>
   <sheets>
     <sheet name="FF Code Base" sheetId="1" r:id="rId1"/>
-    <sheet name="TES Simulink Code" sheetId="2" r:id="rId2"/>
-    <sheet name="MATLAB App" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Problem Description</t>
   </si>
@@ -67,7 +65,28 @@
     <t>The scaling associated with transfering data from wall/base to the particle domain was incorrect. Initial scaling should use prototype parameters and the scaling used to transfer information to particle domain should use the model parameters.</t>
   </si>
   <si>
+    <t>TES.m</t>
+  </si>
+  <si>
     <t>TES.m, FF.m</t>
+  </si>
+  <si>
+    <t>Outlet temperature increasing in time durring charging and holding modes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TES.m </t>
+  </si>
+  <si>
+    <t>g2 needs to be negative</t>
+  </si>
+  <si>
+    <t>Temp distribution goes unstable after a certain period of time</t>
+  </si>
+  <si>
+    <t>Constant for BC1 contribution was being computed incorrectly in "computeBCNow()"</t>
+  </si>
+  <si>
+    <t>Droop characteristic not captured in discharge mode</t>
   </si>
 </sst>
 </file>
@@ -423,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C52C9A-ABED-8249-94C9-614CBC84848F}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -484,36 +503,55 @@
         <v>44795</v>
       </c>
       <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44798</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44798</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44798</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44798</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44798</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01C81FF-A0E8-AD42-AA09-E9D850451A4F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AAB735-215D-3948-BACD-B6A65EB530F0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding enclosure radiation model to base code
</commit_message>
<xml_diff>
--- a/TES Code Error Log.xlsx
+++ b/TES Code Error Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\PhD Research\GranularFunnelFlowModeling\GitFiles\GranularFunnelFlowModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD0EFF7-90C4-4260-806C-4779FD8A7ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F91DC5C-B25E-43D6-BC01-6A7935C95736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
+    <workbookView xWindow="690" yWindow="315" windowWidth="21000" windowHeight="15600" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
   </bookViews>
   <sheets>
     <sheet name="FF Code Base" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Problem Description</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Relevant Code</t>
   </si>
   <si>
+    <t>FF.m</t>
+  </si>
+  <si>
     <t>FF_test.m</t>
   </si>
   <si>
@@ -87,6 +90,9 @@
   </si>
   <si>
     <t>Droop characteristic not captured in discharge mode</t>
+  </si>
+  <si>
+    <t>Temperatures and fluxes in ER model are negative</t>
   </si>
 </sst>
 </file>
@@ -442,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C52C9A-ABED-8249-94C9-614CBC84848F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -486,7 +492,7 @@
         <v>44789</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -494,16 +500,16 @@
         <v>44795</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>44795</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,16 +517,16 @@
         <v>44798</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1">
         <v>44798</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,16 +534,16 @@
         <v>44798</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <v>44798</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,10 +551,21 @@
         <v>44798</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44802</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ER working within FF for multi-cycle simulations
</commit_message>
<xml_diff>
--- a/TES Code Error Log.xlsx
+++ b/TES Code Error Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\PhD Research\GranularFunnelFlowModeling\GitFiles\GranularFunnelFlowModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F91DC5C-B25E-43D6-BC01-6A7935C95736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C009E7-9AFA-460B-B968-BD8A86BBF351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="315" windowWidth="21000" windowHeight="15600" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
   </bookViews>
   <sheets>
     <sheet name="FF Code Base" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Problem Description</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Temperatures and fluxes in ER model are negative</t>
+  </si>
+  <si>
+    <t>Conversion of initial temperatures to Kelvin was done twice</t>
+  </si>
+  <si>
+    <t>Simulation stalls when performing running sequential cycles</t>
+  </si>
+  <si>
+    <t>Seems to be a meshing issue… getting stalled in expm.m</t>
   </si>
 </sst>
 </file>
@@ -448,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C52C9A-ABED-8249-94C9-614CBC84848F}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -564,7 +573,27 @@
       <c r="B7" t="s">
         <v>19</v>
       </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44803</v>
+      </c>
       <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44803</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added small bin model script and changed meshing in FF.m
</commit_message>
<xml_diff>
--- a/TES Code Error Log.xlsx
+++ b/TES Code Error Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive\PhD Research\GranularFunnelFlowModeling\GitFiles\GranularFunnelFlowModeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C009E7-9AFA-460B-B968-BD8A86BBF351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350BBF50-4E21-480F-BD95-6B30CD4AD683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
+    <workbookView xWindow="29490" yWindow="0" windowWidth="21000" windowHeight="15600" xr2:uid="{5753A416-292F-D648-BD72-9121C8A389C5}"/>
   </bookViews>
   <sheets>
     <sheet name="FF Code Base" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Problem Description</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Seems to be a meshing issue… getting stalled in expm.m</t>
+  </si>
+  <si>
+    <t>Charging/discharging final height needs to be more accurate. Bin isn't fully charging and discharging durring cycles.</t>
+  </si>
+  <si>
+    <t>Oscilations in temp profile are causing large temperature droops at the start of discharge</t>
   </si>
 </sst>
 </file>
@@ -457,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C52C9A-ABED-8249-94C9-614CBC84848F}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -593,7 +599,32 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="1">
+        <v>44803</v>
+      </c>
       <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44804</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44804</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>